<commit_message>
Solve in Excel 2013 for correct solution
</commit_message>
<xml_diff>
--- a/optimisation/hw/hw3/hw3_3b.xlsx
+++ b/optimisation/hw/hw3/hw3_3b.xlsx
@@ -1,92 +1,112 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jleach1\Documents\icl\optimisation\hw\hw3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="330" windowWidth="22755" windowHeight="10260"/>
+    <workbookView xWindow="1170" yWindow="330" windowWidth="13950" windowHeight="8085" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Linearity Report 1" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$8:$F$9</definedName>
-    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$8:$F$8</definedName>
-    <definedName name="solver_lhs10" localSheetId="0" hidden="1">Sheet1!$B$41</definedName>
-    <definedName name="solver_lhs11" localSheetId="0" hidden="1">Sheet1!$B$42</definedName>
-    <definedName name="solver_lhs12" localSheetId="0" hidden="1">Sheet1!$B$43</definedName>
-    <definedName name="solver_lhs13" localSheetId="0" hidden="1">Sheet1!$B$44</definedName>
-    <definedName name="solver_lhs14" localSheetId="0" hidden="1">Sheet1!$B$46</definedName>
-    <definedName name="solver_lhs15" localSheetId="0" hidden="1">Sheet1!$B$48</definedName>
-    <definedName name="solver_lhs16" localSheetId="0" hidden="1">Sheet1!$B$51</definedName>
-    <definedName name="solver_lhs17" localSheetId="0" hidden="1">Sheet1!$B$52</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$29</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$B$30</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$B$31</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!$B$32</definedName>
-    <definedName name="solver_lhs6" localSheetId="0" hidden="1">Sheet1!$B$35</definedName>
-    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Sheet1!$B$36</definedName>
-    <definedName name="solver_lhs8" localSheetId="0" hidden="1">Sheet1!$B$37</definedName>
-    <definedName name="solver_lhs9" localSheetId="0" hidden="1">Sheet1!$B$38</definedName>
-    <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">17</definedName>
-    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$B$18</definedName>
-    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
-    <definedName name="solver_rel1" localSheetId="0" hidden="1">5</definedName>
-    <definedName name="solver_rel10" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel11" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel12" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel13" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel14" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel15" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel16" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel17" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel5" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel8" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">binary</definedName>
-    <definedName name="solver_rhs10" localSheetId="0" hidden="1">Sheet1!$C$41</definedName>
-    <definedName name="solver_rhs11" localSheetId="0" hidden="1">Sheet1!$C$42</definedName>
-    <definedName name="solver_rhs12" localSheetId="0" hidden="1">Sheet1!$C$43</definedName>
-    <definedName name="solver_rhs13" localSheetId="0" hidden="1">Sheet1!$C$44</definedName>
-    <definedName name="solver_rhs14" localSheetId="0" hidden="1">Sheet1!$C$46</definedName>
-    <definedName name="solver_rhs15" localSheetId="0" hidden="1">Sheet1!$C$48</definedName>
-    <definedName name="solver_rhs16" localSheetId="0" hidden="1">Sheet1!$C$51</definedName>
-    <definedName name="solver_rhs17" localSheetId="0" hidden="1">Sheet1!$C$52</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!$C$29</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$C$30</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Sheet1!$C$31</definedName>
-    <definedName name="solver_rhs5" localSheetId="0" hidden="1">Sheet1!$C$32</definedName>
-    <definedName name="solver_rhs6" localSheetId="0" hidden="1">Sheet1!$C$35</definedName>
-    <definedName name="solver_rhs7" localSheetId="0" hidden="1">Sheet1!$C$36</definedName>
-    <definedName name="solver_rhs8" localSheetId="0" hidden="1">Sheet1!$C$37</definedName>
-    <definedName name="solver_rhs9" localSheetId="0" hidden="1">Sheet1!$C$38</definedName>
-    <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_tim" localSheetId="0" hidden="1">300</definedName>
-    <definedName name="solver_tol" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">Sheet1!$B$8:$F$9</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">500</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sheet1!$B$29</definedName>
+    <definedName name="solver_lhs10" localSheetId="1" hidden="1">Sheet1!$B$42</definedName>
+    <definedName name="solver_lhs11" localSheetId="1" hidden="1">Sheet1!$B$43</definedName>
+    <definedName name="solver_lhs12" localSheetId="1" hidden="1">Sheet1!$B$44</definedName>
+    <definedName name="solver_lhs13" localSheetId="1" hidden="1">Sheet1!$B$46</definedName>
+    <definedName name="solver_lhs14" localSheetId="1" hidden="1">Sheet1!$B$48</definedName>
+    <definedName name="solver_lhs15" localSheetId="1" hidden="1">Sheet1!$B$51</definedName>
+    <definedName name="solver_lhs16" localSheetId="1" hidden="1">Sheet1!$B$52</definedName>
+    <definedName name="solver_lhs17" localSheetId="1" hidden="1">Sheet1!$B$8:$F$8</definedName>
+    <definedName name="solver_lhs18" localSheetId="1" hidden="1">Sheet1!$B$44</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sheet1!$B$30</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">Sheet1!$B$31</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">Sheet1!$B$32</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">Sheet1!$B$35</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">Sheet1!$B$36</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">Sheet1!$B$37</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">Sheet1!$B$38</definedName>
+    <definedName name="solver_lhs9" localSheetId="1" hidden="1">Sheet1!$B$41</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">17</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Sheet1!$B$18</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.0000000000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel10" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel11" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel12" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel13" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel14" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel15" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel16" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel17" localSheetId="1" hidden="1">5</definedName>
+    <definedName name="solver_rel18" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel7" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel8" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel9" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">Sheet1!$C$29</definedName>
+    <definedName name="solver_rhs10" localSheetId="1" hidden="1">Sheet1!$C$42</definedName>
+    <definedName name="solver_rhs11" localSheetId="1" hidden="1">Sheet1!$C$43</definedName>
+    <definedName name="solver_rhs12" localSheetId="1" hidden="1">Sheet1!$C$44</definedName>
+    <definedName name="solver_rhs13" localSheetId="1" hidden="1">Sheet1!$C$46</definedName>
+    <definedName name="solver_rhs14" localSheetId="1" hidden="1">Sheet1!$C$48</definedName>
+    <definedName name="solver_rhs15" localSheetId="1" hidden="1">Sheet1!$C$51</definedName>
+    <definedName name="solver_rhs16" localSheetId="1" hidden="1">Sheet1!$C$52</definedName>
+    <definedName name="solver_rhs17" localSheetId="1" hidden="1">binary</definedName>
+    <definedName name="solver_rhs18" localSheetId="1" hidden="1">Sheet1!$C$44</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">Sheet1!$C$30</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">Sheet1!$C$31</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">Sheet1!$C$32</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">Sheet1!$C$35</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">Sheet1!$C$36</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">Sheet1!$C$37</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">Sheet1!$C$38</definedName>
+    <definedName name="solver_rhs9" localSheetId="1" hidden="1">Sheet1!$C$41</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">600</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="96">
   <si>
     <t>Product</t>
   </si>
@@ -191,17 +211,201 @@
   </si>
   <si>
     <t>M-notation</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 15.0 Linearity Report</t>
+  </si>
+  <si>
+    <t>Worksheet: [hw3_3b.xlsx]Sheet1</t>
+  </si>
+  <si>
+    <t>Report Created: 09/12/2015 08:04:08</t>
+  </si>
+  <si>
+    <t>Objective Cell (Max)</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Original Value</t>
+  </si>
+  <si>
+    <t>Final Value</t>
+  </si>
+  <si>
+    <t>Linear Function</t>
+  </si>
+  <si>
+    <t>Variable Cells</t>
+  </si>
+  <si>
+    <t>Occurs Linearly</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>Cell Value</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>$B$18</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>$B$8</t>
+  </si>
+  <si>
+    <t>$C$8</t>
+  </si>
+  <si>
+    <t>$D$8</t>
+  </si>
+  <si>
+    <t>$E$8</t>
+  </si>
+  <si>
+    <t>$F$8</t>
+  </si>
+  <si>
+    <t>Decisions Switching Variable</t>
+  </si>
+  <si>
+    <t>$B$9</t>
+  </si>
+  <si>
+    <t>$C$9</t>
+  </si>
+  <si>
+    <t>$D$9</t>
+  </si>
+  <si>
+    <t>$E$9</t>
+  </si>
+  <si>
+    <t>$F$9</t>
+  </si>
+  <si>
+    <t>Quantities Switching Variable</t>
+  </si>
+  <si>
+    <t>$B$29</t>
+  </si>
+  <si>
+    <t>$B$29&gt;=$C$29</t>
+  </si>
+  <si>
+    <t>$B$30</t>
+  </si>
+  <si>
+    <t>$B$30&gt;=$C$30</t>
+  </si>
+  <si>
+    <t>$B$31</t>
+  </si>
+  <si>
+    <t>$B$31&gt;=$C$31</t>
+  </si>
+  <si>
+    <t>$B$32</t>
+  </si>
+  <si>
+    <t>$B$32&gt;=$C$32</t>
+  </si>
+  <si>
+    <t>$B$35</t>
+  </si>
+  <si>
+    <t>$B$35&lt;=$C$35</t>
+  </si>
+  <si>
+    <t>$B$36</t>
+  </si>
+  <si>
+    <t>$B$36&lt;=$C$36</t>
+  </si>
+  <si>
+    <t>$B$37</t>
+  </si>
+  <si>
+    <t>$B$37&lt;=$C$37</t>
+  </si>
+  <si>
+    <t>$B$38</t>
+  </si>
+  <si>
+    <t>$B$38&lt;=$C$38</t>
+  </si>
+  <si>
+    <t>$B$41</t>
+  </si>
+  <si>
+    <t>$B$41&lt;=$C$41</t>
+  </si>
+  <si>
+    <t>$B$42</t>
+  </si>
+  <si>
+    <t>$B$42&lt;=$C$42</t>
+  </si>
+  <si>
+    <t>$B$43</t>
+  </si>
+  <si>
+    <t>$B$43&lt;=$C$43</t>
+  </si>
+  <si>
+    <t>$B$44</t>
+  </si>
+  <si>
+    <t>$B$44&lt;=$C$44</t>
+  </si>
+  <si>
+    <t>$B$46</t>
+  </si>
+  <si>
+    <t>$B$46&lt;=$C$46</t>
+  </si>
+  <si>
+    <t>$B$48</t>
+  </si>
+  <si>
+    <t>$B$48&lt;=$C$48</t>
+  </si>
+  <si>
+    <t>$B$51</t>
+  </si>
+  <si>
+    <t>$B$51&lt;=$C$51</t>
+  </si>
+  <si>
+    <t>$B$52</t>
+  </si>
+  <si>
+    <t>$B$52&lt;=$C$52</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +436,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -247,7 +459,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -298,45 +510,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -344,6 +598,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -390,7 +652,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -422,9 +684,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -456,6 +719,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -631,24 +895,579 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="22">
+        <v>0</v>
+      </c>
+      <c r="E8" s="22">
+        <v>0</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="24">
+        <v>0</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="24">
+        <v>0</v>
+      </c>
+      <c r="E14" s="24">
+        <v>0</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="24">
+        <v>0</v>
+      </c>
+      <c r="E15" s="24">
+        <v>0</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="24">
+        <v>0</v>
+      </c>
+      <c r="E16" s="24">
+        <v>0</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="24">
+        <v>0</v>
+      </c>
+      <c r="E17" s="24">
+        <v>0</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="24">
+        <v>0</v>
+      </c>
+      <c r="E18" s="24">
+        <v>0</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="24">
+        <v>0</v>
+      </c>
+      <c r="E19" s="24">
+        <v>0</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="24">
+        <v>0</v>
+      </c>
+      <c r="E20" s="24">
+        <v>0</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="24">
+        <v>0</v>
+      </c>
+      <c r="E21" s="24">
+        <v>0</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="22">
+        <v>0</v>
+      </c>
+      <c r="E22" s="22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="24">
+        <v>0</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="24">
+        <v>0</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="24">
+        <v>0</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="24">
+        <v>0</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="21"/>
+      <c r="D31" s="24">
+        <v>0</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="21"/>
+      <c r="D32" s="24">
+        <v>0</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="D33" s="24">
+        <v>0</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="21"/>
+      <c r="D34" s="24">
+        <v>0</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="24">
+        <v>0</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="24">
+        <v>0</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="24">
+        <v>0</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="24">
+        <v>0</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="24">
+        <v>0</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="24">
+        <v>0</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="24">
+        <v>0</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="22">
+        <v>0</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="34" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -657,7 +1476,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -674,7 +1493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
@@ -691,7 +1510,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -708,7 +1527,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
@@ -725,7 +1544,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -737,47 +1556,47 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="6">
-        <v>0.99998849561881464</v>
+        <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>0.9999923304115429</v>
+        <v>1</v>
       </c>
       <c r="D8" s="6">
-        <v>1.1504381185638389E-5</v>
+        <v>1</v>
       </c>
       <c r="E8" s="6">
-        <v>7.6695884571043038E-6</v>
+        <v>0</v>
       </c>
       <c r="F8" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="6">
-        <v>3834.7957285177431</v>
+        <v>0</v>
       </c>
       <c r="C9" s="6">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="D9" s="6">
-        <v>11504.381185644761</v>
+        <v>12500</v>
       </c>
       <c r="E9" s="6">
-        <v>7669.5884570815006</v>
+        <v>0</v>
       </c>
       <c r="F9" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -786,85 +1605,85 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="6">
         <f>B9*B4</f>
-        <v>268435.700996242</v>
+        <v>0</v>
       </c>
       <c r="C14" s="6">
         <f>C9*C4</f>
-        <v>0</v>
+        <v>900000</v>
       </c>
       <c r="D14" s="6">
         <f>D9*D4</f>
-        <v>1035394.3067080285</v>
+        <v>1125000</v>
       </c>
       <c r="E14" s="6">
         <f>E9*E4</f>
-        <v>613567.07656652003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="17">
         <f>B8*B3</f>
-        <v>49999.424780940732</v>
+        <v>0</v>
       </c>
       <c r="C15" s="11">
         <f>C8*C3</f>
-        <v>39999.693216461717</v>
+        <v>40000</v>
       </c>
       <c r="D15" s="11">
         <f>D8*D3</f>
-        <v>0.80530668299468722</v>
+        <v>70000</v>
       </c>
       <c r="E15" s="11">
         <f>E8*E3</f>
-        <v>0.46017530742625823</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickTop="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="10">
         <f>B14-B15</f>
-        <v>218436.27621530127</v>
+        <v>0</v>
       </c>
       <c r="C16" s="10">
         <f>C14-C15</f>
-        <v>-39999.693216461717</v>
+        <v>860000</v>
       </c>
       <c r="D16" s="10">
         <f>D14-D15</f>
-        <v>1035393.5014013456</v>
+        <v>1055000</v>
       </c>
       <c r="E16" s="10">
         <f>E14-E15</f>
-        <v>613566.61639121256</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="9">
-        <f>SUM(B16:E16)</f>
-        <v>1827396.7007913976</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <f>(B9*B4+C9*C4+D9*D4+E9*E4)-(B8*B3+C8*C3+D8*D3+E8*E3)</f>
+        <v>1915000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D19" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -872,325 +1691,328 @@
         <v>26</v>
       </c>
       <c r="E20" s="6">
-        <v>1000000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="16">
         <f>B8</f>
-        <v>0.99998849561881464</v>
+        <v>0</v>
       </c>
       <c r="C22" s="16"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="16">
         <f>C8</f>
-        <v>0.9999923304115429</v>
+        <v>1</v>
       </c>
       <c r="C23" s="16"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="16">
         <f>D8</f>
-        <v>1.1504381185638389E-5</v>
+        <v>1</v>
       </c>
       <c r="C24" s="16"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="16">
         <f>E8</f>
-        <v>7.6695884571043038E-6</v>
+        <v>0</v>
       </c>
       <c r="C25" s="16"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="16">
         <f>F8</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C26" s="16"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="E27" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="16">
         <f>B9</f>
-        <v>3834.7957285177431</v>
+        <v>0</v>
       </c>
       <c r="C29" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="16">
         <f>C9</f>
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="C30" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="16">
         <f>D9</f>
-        <v>11504.381185644761</v>
+        <v>12500</v>
       </c>
       <c r="C31" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="16">
         <f>E9</f>
-        <v>7669.5884570815006</v>
+        <v>0</v>
       </c>
       <c r="C32" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>1</v>
       </c>
       <c r="B35" s="16">
         <f>B9</f>
-        <v>3834.7957285177431</v>
+        <v>0</v>
       </c>
       <c r="C35" s="16">
         <f>B8*E20</f>
-        <v>999988495.61881459</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>2</v>
       </c>
       <c r="B36" s="16">
         <f>C9</f>
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="C36" s="16">
         <f>C8*E20</f>
-        <v>999992330.41154289</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>3</v>
       </c>
       <c r="B37" s="16">
         <f>D9</f>
-        <v>11504.381185644761</v>
+        <v>12500</v>
       </c>
       <c r="C37" s="16">
         <f>D8*E20</f>
-        <v>11504.381185638389</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>4</v>
       </c>
       <c r="B38" s="16">
         <f>E9</f>
-        <v>7669.5884570815006</v>
+        <v>0</v>
       </c>
       <c r="C38" s="16">
         <f>E8*E20</f>
-        <v>7669.5884571043034</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="6">
         <f>B9</f>
-        <v>3834.7957285177431</v>
+        <v>0</v>
       </c>
       <c r="C41" s="6">
         <f>B5</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B42" s="6">
         <f>C9</f>
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="C42" s="6">
         <f>C5</f>
         <v>15000</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B43" s="6">
         <f>D9</f>
-        <v>11504.381185644761</v>
+        <v>12500</v>
       </c>
       <c r="C43" s="6">
         <f>D5</f>
         <v>12500</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B44" s="6">
         <f>E9</f>
-        <v>7669.5884570815006</v>
+        <v>0</v>
       </c>
       <c r="C44" s="6">
         <f>E5</f>
         <v>9000</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B46" s="6">
         <f>B8+C8+D8+E8</f>
-        <v>2.0000000000000004</v>
+        <v>2</v>
       </c>
       <c r="C46" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B48" s="6">
         <f>D8</f>
-        <v>1.1504381185638389E-5</v>
+        <v>1</v>
       </c>
       <c r="C48" s="6">
         <f>B8+C8</f>
-        <v>1.9999808260303575</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B51" s="6">
         <f>B9+C9</f>
-        <v>3834.7957285177431</v>
+        <v>15000</v>
       </c>
       <c r="C51" s="6">
         <f>20000+(E20*F8)</f>
-        <v>500020000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B52" s="1">
         <f>D9+E9</f>
-        <v>19173.969642726261</v>
+        <v>12500</v>
       </c>
       <c r="C52" s="1">
         <f>20000+(E20*(1-F8))</f>
-        <v>500020000</v>
+        <v>1020000</v>
       </c>
     </row>
   </sheetData>
@@ -1199,25 +2021,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>